<commit_message>
Processed Results - mean and median increase
</commit_message>
<xml_diff>
--- a/Processed Results/Mi 9T/Accelerometer/Accelerometer - Processed.xlsx
+++ b/Processed Results/Mi 9T/Accelerometer/Accelerometer - Processed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luuk1\Desktop\Bachelor Project\BachelorProject\Processed Results\Mi 9T\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luuk1\Desktop\Bachelor Project\BachelorProject\Processed Results\Mi 9T\Accelerometer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8C25CF-3FA4-4A13-A1CA-2168631FCE1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04356730-8A5B-4712-A5A0-28FD26C41984}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BD96B59B-3C3E-42C2-91CD-DAE8785DB1E9}"/>
+    <workbookView xWindow="160" yWindow="240" windowWidth="9990" windowHeight="9830" xr2:uid="{BD96B59B-3C3E-42C2-91CD-DAE8785DB1E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="14">
   <si>
     <t>Mean line</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Relative std</t>
+  </si>
+  <si>
+    <t>Mean increase</t>
+  </si>
+  <si>
+    <t>Median increase</t>
   </si>
 </sst>
 </file>
@@ -2387,10 +2393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78FE0459-F6C0-45BE-AD60-56F63431C3F0}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E16" sqref="D15:E16"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2603,7 +2609,7 @@
         <v>0.87210580895007472</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -2611,23 +2617,37 @@
         <v>101.94976800000001</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="1">
         <v>101.79071999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>3</v>
       </c>
       <c r="B19" s="1">
         <v>101.313576</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D19" s="1">
+        <f>((102.130022 / 95.321842) * 100) - 100</f>
+        <v>7.1423084753230057</v>
+      </c>
+      <c r="F19">
+        <f xml:space="preserve"> ((101.949768 / 95.22216) * 100) - 100</f>
+        <v>7.0651705443354871</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -2635,7 +2655,7 @@
         <v>101.313576</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -2643,7 +2663,7 @@
         <v>103.381199999999</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -2651,7 +2671,7 @@
         <v>102.108816</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -2659,7 +2679,7 @@
         <v>102.426912</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -2667,7 +2687,7 @@
         <v>102.108816</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -2675,7 +2695,7 @@
         <v>102.745008</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -2683,7 +2703,7 @@
         <v>103.063104</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -2691,7 +2711,7 @@
         <v>102.426912</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -2699,7 +2719,7 @@
         <v>102.108816</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -2707,7 +2727,7 @@
         <v>101.94976800000001</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -2715,7 +2735,7 @@
         <v>101.79071999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -2723,7 +2743,7 @@
         <v>102.904056</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B32" s="2"/>
     </row>
   </sheetData>

</xml_diff>